<commit_message>
Small change in VGA docs
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/VGA spec.xlsx
+++ b/2nd gen - 8 bit cpu/VGA spec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Parameter</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>http://martin.hinner.info/vga/timing.html</t>
+  </si>
+  <si>
+    <t>How to interface CPU writes to VRAM and reads from VGA board to the same memory:</t>
+  </si>
+  <si>
+    <t>https://electronics.stackexchange.com/questions/268136/interface-between-two-different-bus-speeds</t>
   </si>
 </sst>
 </file>
@@ -389,14 +395,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -417,16 +423,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>296636</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>84364</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -450,8 +456,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5819775" y="790575"/>
-          <a:ext cx="9563100" cy="1962150"/>
+          <a:off x="6272893" y="2340428"/>
+          <a:ext cx="9603922" cy="1962150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -477,15 +483,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>517071</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -510,8 +516,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5819775" y="2886075"/>
-          <a:ext cx="10001250" cy="7581900"/>
+          <a:off x="6300107" y="4408714"/>
+          <a:ext cx="10044793" cy="7581900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -820,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +871,7 @@
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>25175</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -879,27 +885,33 @@
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>31469</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>640</v>
       </c>
       <c r="D6" s="7"/>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="7"/>
@@ -908,7 +920,7 @@
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>31778</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -919,7 +931,7 @@
       <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -930,7 +942,7 @@
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>3813</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -941,7 +953,7 @@
       <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>1907</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -952,7 +964,7 @@
       <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>25422</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1024,7 +1036,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="12">
@@ -1035,7 +1047,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="16">
         <f>C21/$C$19</f>
         <v>16.011328770356386</v>
@@ -1045,7 +1057,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="12">
@@ -1056,7 +1068,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="16">
         <f>C23/$C$19</f>
         <v>95.992447486429086</v>
@@ -1066,7 +1078,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="12">
@@ -1077,7 +1089,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="16">
         <f>C25/$C$19</f>
         <v>48.00881126583274</v>
@@ -1276,7 +1288,7 @@
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C51" s="12">
@@ -1287,7 +1299,7 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="23"/>
+      <c r="B52" s="25"/>
       <c r="C52" s="16">
         <f>C51/$C$48</f>
         <v>10.00692302851029</v>
@@ -1297,7 +1309,7 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C53" s="12">
@@ -1308,7 +1320,7 @@
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="23"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="16">
         <f>C53/$C$48</f>
         <v>2.013971930266222</v>
@@ -1318,7 +1330,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="12">
@@ -1329,7 +1341,7 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="23"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="16">
         <f>C55/$C$48</f>
         <v>32.978790358109386</v>
@@ -1402,10 +1414,11 @@
     <hyperlink ref="F3" r:id="rId5" location="Specifications"/>
     <hyperlink ref="D42" r:id="rId6" tooltip="Millisecond" display="https://en.wikipedia.org/wiki/Millisecond"/>
     <hyperlink ref="F2" r:id="rId7"/>
+    <hyperlink ref="F6" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
CSCompiler - refactoring (not finished)
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/VGA spec.xlsx
+++ b/2nd gen - 8 bit cpu/VGA spec.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Parameter</t>
   </si>
@@ -198,6 +197,39 @@
   <si>
     <t>https://electronics.stackexchange.com/questions/268136/interface-between-two-different-bus-speeds</t>
   </si>
+  <si>
+    <t>Horizontal:</t>
+  </si>
+  <si>
+    <t>Active:</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Blanking:</t>
+  </si>
+  <si>
+    <t>Vertical:</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Although 480 lines are displayed, 521 lines are act</t>
+  </si>
+  <si>
+    <t>Vert blanking:</t>
+  </si>
+  <si>
+    <t>521 x 6,6 us:</t>
+  </si>
+  <si>
+    <t>Total blanking / frame:</t>
+  </si>
+  <si>
+    <t>Total time / frame:</t>
+  </si>
 </sst>
 </file>
 
@@ -206,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +276,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242729"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -349,11 +394,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -404,10 +450,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -826,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1424,24 +1473,160 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>25.17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>31.77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <f>B4-B3</f>
+        <v>6.5999999999999979</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="26">
+        <f>B5/B4</f>
+        <v>0.20774315391879125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>15.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <v>16.783999999999999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <f>B12-B11</f>
+        <v>1.5339999999999989</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="26">
+        <f>B13/B12</f>
+        <v>9.1396568160152472E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <f>521 * 0.0000066</f>
+        <v>3.4386E-3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22">
+        <v>1.534E-3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24">
+        <f>B21+B22</f>
+        <v>4.9725999999999998E-3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="26">
+        <f>B24/B25</f>
+        <v>0.29627025738798857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25">
+        <v>1.6784E-2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>